<commit_message>
Broke down milestones, gave the game a title worked and worked on game
I broke down each milestone into smaller segments and i gave mt game a title, Cabin Boy Fowx is what i will be calling my pirate adventure. I finished the basic Crystal Voyager model(however not finishe, will be worked on at a later date). I started creating the ocean and for now put the Roll a Ball movement script onto my ship, which obviously didn't work because it is impossible to move my ship due to current physics, i am hoping once im able to make the ship float i will be able to make this script work, once i am succesfully able to move my ship i will give it a more advanced yet simple movement code.
</commit_message>
<xml_diff>
--- a/GAM403-A2_Milestones_Ritikh_Prasad.xlsx
+++ b/GAM403-A2_Milestones_Ritikh_Prasad.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thera\Desktop\Uni\GAM403_A2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thera\Desktop\Uni\GAM403_A2\GAM403_A2_Ritikh_Prasad\GAM403_A2_Ritikh_Prasad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E6AF41-75CC-4C41-AEEF-01CB0AFF8643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B14D52-444F-4759-BE3A-1C8F922DC334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{2AD2CF00-CD03-4335-9EA3-956C0D57C64D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Milestone</t>
   </si>
@@ -64,6 +64,18 @@
       </rPr>
       <t xml:space="preserve">Milestones  </t>
     </r>
+  </si>
+  <si>
+    <t>Days Left</t>
+  </si>
+  <si>
+    <t>Building the first playable pirate ship</t>
+  </si>
+  <si>
+    <t>very time consuming using only Unity preset game objects. (start date -30/3/2020)</t>
+  </si>
+  <si>
+    <t>Creating enemy AI</t>
   </si>
   <si>
     <r>
@@ -95,11 +107,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Project Name</t>
+      <t>Cabin Boy Fowx</t>
     </r>
-  </si>
-  <si>
-    <t>Days Left</t>
   </si>
   <si>
     <r>
@@ -114,41 +123,56 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Firstname Lastname</t>
+      <t>Ritikh Prasad</t>
     </r>
   </si>
   <si>
-    <t>Building the first playable pirate ship</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Building the first pirate ship called the 'Crystal Voyager'. </t>
-  </si>
-  <si>
-    <t>Player controls and ultimate attack</t>
-  </si>
-  <si>
-    <t>Completing the controls for the player character, for example movement, attacks and gimmicks and implementing the Crystal Voyager's ultimate attack 'Crystal Fury'.</t>
-  </si>
-  <si>
-    <t>Building enemy pirate ship</t>
-  </si>
-  <si>
-    <t>very time consuming using only Unity preset game objects. (start date -30/3/2020)</t>
-  </si>
-  <si>
-    <t>Ruffian (enemy) AI</t>
-  </si>
-  <si>
-    <t>Anchor and dock ship mechanic</t>
-  </si>
-  <si>
-    <t>Implementing enemy AI to locate and track you down.</t>
-  </si>
-  <si>
-    <t>Building the enemy pirate ship 'Ruffian'.</t>
-  </si>
-  <si>
-    <t>Implement an anchor mechanic so youre ship can rotate in a fixed position and a docking mechanic which allows you to save the game at your starting dock.</t>
+    <t>Player controls</t>
+  </si>
+  <si>
+    <t>Create ocean and land</t>
+  </si>
+  <si>
+    <t>Create placeholder ocean and land</t>
+  </si>
+  <si>
+    <t>Refine code</t>
+  </si>
+  <si>
+    <t>Create a more advanced but simple PlayerControl script</t>
+  </si>
+  <si>
+    <t>Refine Crystal Voyager</t>
+  </si>
+  <si>
+    <t>Finish creating the Crystal Voyager</t>
+  </si>
+  <si>
+    <t>Create 'Kill Switch' code</t>
+  </si>
+  <si>
+    <t>Create the code for the Kill Switch which is the ship's special attack</t>
+  </si>
+  <si>
+    <t>Code Crystal Voyager's Kill Switch</t>
+  </si>
+  <si>
+    <t>Create the code for 'Crystal Fury', the Crystal Voyager's special attack/Kill Switch</t>
+  </si>
+  <si>
+    <t>Animate Crystal Fury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build the first pirate ship called the 'Crystal Voyager'. </t>
+  </si>
+  <si>
+    <t>Code the controls for the player character, i.e movement and cannon fire</t>
+  </si>
+  <si>
+    <t>Code and attach enemy AI to a placeholder enemy to test and refine code before creating the enemy ship ('Ruffian")</t>
+  </si>
+  <si>
+    <t>Create the animation for the Crystal Fury Kill Switch</t>
   </si>
 </sst>
 </file>
@@ -777,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA462C77-ECFC-40AE-BD92-9F45B89E8D15}">
   <dimension ref="A2:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,10 +824,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="23"/>
@@ -820,7 +844,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>4</v>
@@ -832,97 +856,103 @@
     </row>
     <row r="5" spans="1:10" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2">
         <v>43921</v>
       </c>
       <c r="E5" s="19">
         <f t="shared" ref="E5:E36" ca="1" si="0">IF(D5&lt;&gt;"",D5-TODAY(),"")</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F5" s="2">
         <v>43921</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D6" s="5">
         <v>43921</v>
       </c>
       <c r="E6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="5"/>
+        <v>-1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>43922</v>
+      </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2">
         <v>43922</v>
       </c>
       <c r="E7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8" s="5">
         <v>43922</v>
       </c>
       <c r="E8" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>16</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>19</v>
       </c>
       <c r="D9" s="2">
         <v>43923</v>
       </c>
       <c r="E9" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="20" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -932,8 +962,12 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="19" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -943,8 +977,12 @@
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="20" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -954,8 +992,12 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="19" t="str">
         <f t="shared" ca="1" si="0"/>

</xml_diff>